<commit_message>
Removed a few columns in order to reflect changes in database (courses do not need to have region listed)
</commit_message>
<xml_diff>
--- a/smartgrid/dbdata/Spreadsheets/Courses.xlsx
+++ b/smartgrid/dbdata/Spreadsheets/Courses.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37900" yWindow="-5540" windowWidth="12460" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="37905" yWindow="-5535" windowWidth="12465" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
   <si>
     <t>X423</t>
   </si>
@@ -295,13 +295,16 @@
   </si>
   <si>
     <t>To be used by ERG students only preparing for qualifying exams. </t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -412,6 +415,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -737,793 +745,805 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="25.75" customWidth="1"/>
+    <col min="3" max="3" width="33.125" customWidth="1"/>
+    <col min="4" max="4" width="17.75" customWidth="1"/>
+    <col min="5" max="5" width="19.875" customWidth="1"/>
+    <col min="6" max="6" width="17.875" customWidth="1"/>
+    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="8" max="8" width="14.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="2" t="s">
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s">
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="2" t="s">
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="2">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2" t="s">
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2" t="s">
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2" t="s">
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="2">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="5">
-        <v>2</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="2" t="s">
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="5">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="2">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="5">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="2" t="s">
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="2">
-        <v>3</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="5">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="2" t="s">
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="5">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="5">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="2" t="s">
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="2">
-        <v>3</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="5">
-        <v>2</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="8" t="s">
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="2">
-        <v>3</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="5">
-        <v>2</v>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G17" s="5">
-        <v>1</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="2">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="5">
-        <v>2</v>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G18" s="5">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="2">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="5">
-        <v>2</v>
+      <c r="E19" s="2">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G19" s="5">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="2">
-        <v>3</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="5">
-        <v>2</v>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G20" s="5">
-        <v>1</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="2">
-        <v>3</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="5">
-        <v>2</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2" t="s">
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="2">
-        <v>3</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="5">
-        <v>2</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="2" t="s">
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="5">
+        <v>2</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="2">
-        <v>3</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="5">
-        <v>2</v>
-      </c>
-      <c r="G23" s="2">
-        <v>1</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="2" t="s">
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="2">
-        <v>3</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="5">
-        <v>2</v>
-      </c>
-      <c r="G24" s="2">
-        <v>1</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="2" t="s">
+      <c r="E24" s="2">
+        <v>3</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="5">
+        <v>2</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="5">
-        <v>2</v>
-      </c>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="2" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="2">
-        <v>3</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="5">
-        <v>2</v>
+      <c r="E26" s="2">
+        <v>3</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G26" s="5">
-        <v>1</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2">
-        <v>3</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="5">
-        <v>2</v>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2">
+        <v>3</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G27" s="5">
-        <v>1</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="2">
-        <v>3</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="5">
-        <v>2</v>
+      <c r="E28" s="2">
+        <v>3</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G28" s="5">
-        <v>1</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="2">
-        <v>3</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="5">
-        <v>2</v>
+      <c r="E29" s="2">
+        <v>3</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G29" s="5">
-        <v>1</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="B30" s="10"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="B31" s="11"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="C30" s="10"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="C31" s="11"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C28" r:id="rId1"/>
+    <hyperlink ref="D28" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>